<commit_message>
0.1.07 - Change member load addition
</commit_message>
<xml_diff>
--- a/Source/Excel/Simple_Piperack/RC_Members_01.xlsx
+++ b/Source/Excel/Simple_Piperack/RC_Members_01.xlsx
@@ -519,14 +519,15 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="8" style="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="1"/>
+    <col min="3" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="8.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
     <col min="6" max="6" width="8.5703125" style="4" customWidth="1"/>
     <col min="7" max="7" width="4.85546875" style="4" customWidth="1"/>

</xml_diff>